<commit_message>
configuracion aps en vsz
</commit_message>
<xml_diff>
--- a/media/output.xlsx
+++ b/media/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,27 +424,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ap_name 1</t>
+          <t>BUESCAP01</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Ip 1</t>
+          <t>192.168.112.50</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>3C:46:A1:25:78:90</t>
+          <t>3C:46:A1:25:46:20</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>122379003272</t>
+          <t>122379002601</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Descripcion 1</t>
+          <t>SAN TELMO 1</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -456,27 +456,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ap_name 2</t>
+          <t>BUESCAP02</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ip 2</t>
+          <t>192.168.112.51</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>3C:46:A1:25:46:20</t>
+          <t>3C:46:A1:25:78:90</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>122379002601</t>
+          <t>122379003272</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Descripcion 2</t>
+          <t>SAN TELMO 2</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -488,27 +488,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ap_name 3</t>
+          <t>BUESCAP03</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ip 3</t>
+          <t>192.168.112.52</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3C:46:A1:25:46:20</t>
+          <t>3C:46:A1:25:4B:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>122379002601</t>
+          <t>122379002817</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Descripcion 3</t>
+          <t>SAN TELMO 3</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -520,64 +520,1202 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ap_name 4</t>
+          <t>BUESCAP04</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ip 4</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>3C:46:A1:25:78:90</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>122379003272</t>
+          <t>192.168.112.53</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Descripcion 4</t>
+          <t>SAN TELMO 4</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>en uso</t>
+          <t>libre</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ap_name 5</t>
+          <t>BUESCAP05</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ip 5</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>3C:46:A1:25:46:20</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>122379002601</t>
+          <t>192.168.112.54</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Descripcion 5</t>
+          <t>SAN TELMO 5</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>en uso</t>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>BUESCAP06</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>192.168.112.55</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>SAN ISIDRO 1</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>BUESCAP07</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>192.168.112.56</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>SAN ISIDRO 2</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>BUESCAP08</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>192.168.112.57</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>SAN ISIDRO 3</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>BUESCAP09</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>192.168.112.58</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>SAN ISIDRO 4</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>BUESCAP10</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>192.168.112.59</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>FOYER SAN ISIDRO</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>BUESCAP11</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>192.168.112.60</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>CREW1</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>BUESCAP12</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>192.168.112.61</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>CREW2</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>BUESCAP13</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>192.168.112.62</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>AUDITORIO</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>BUESCAP14</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>192.168.112.63</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>PELUQUERIA</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>BUESCAP15</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>192.168.112.64</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LOBBY 1</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>BUESCAP16</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>192.168.112.65</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LOBBY 2</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>BUESCAP17</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>192.168.112.66</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LOBBY 3</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>BUESCAP18</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>192.168.112.67</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LOBBY 4</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>BUESCAP19</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>192.168.112.68</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LINK SHERATON</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>BUESCAP20</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>192.168.112.69</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>BAR 1</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>BUESCAP21</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>192.168.112.70</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>BAR 2</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>BUESCAP22</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>192.168.112.71</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>BUONO 1</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>BUESCAP23</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>192.168.112.72</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>BUONO 2</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>BUESCAP24</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>192.168.112.73</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>BUONO 3</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>BUESCAP25</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>192.168.112.74</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>SNACK</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>BUESCAP26</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>192.168.112.75</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>GYM</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>BUESCAP27</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>192.168.112.76</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LA PAMPA 1</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>BUESCAP28</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>192.168.112.77</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LA PAMPA 2</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>BUESCAP29</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>192.168.112.78</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>GOLDEN 1</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>BUESCAP30</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>192.168.112.79</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>GOLDEN 2</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>BUESCAP31</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>192.168.112.80</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>CATALINAS 1</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>BUESCAP32</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>192.168.112.81</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>CATALINAS 2</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>BUESCAP33</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>192.168.112.82</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>FOYER CATALINAS</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>BUESCAP34</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>192.168.112.83</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>FOYER LIBERTADOR 1</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>BUESCAP35</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>192.168.112.84</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>FOYER LIBERTADOR 2</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>BUESCAP36</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>192.168.112.85</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>FOYER LIBERTADOR 3</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>BUESCAP37</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>192.168.112.86</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>FOYER LIBERTADOR 4</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>BUESCAP38</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>192.168.112.87</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>SALON LIBERTADOR 1</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>BUESCAP39</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>192.168.112.88</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>SALON LIBERTADOR 2</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>BUESCAP40</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>192.168.112.89</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>SALON LIBERTADOR 3</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>BUESCAP41</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>192.168.112.90</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>SALON LIBERTADOR 4</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>BUESCAP42</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>192.168.112.91</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>SALON LIBERTADOR 5</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>BUESCAP43</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>192.168.112.92</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>SALON LIBERTADOR 6</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>BUESCAP44</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>192.168.112.93</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>FOYER RETIRO 1</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>BUESCAP45</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>192.168.112.94</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>FOYER RETIRO 2</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>BUESCAP46</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>192.168.112.95</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>SALON RETIRO 1</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>BUESCAP47</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>192.168.112.96</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>SALON RETIRO 2</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>BUESCAP48</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>192.168.112.97</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>SALON RETIRO 3</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>BUESCAP49</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>192.168.112.98</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>SALON RETIRO 4</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>BUESCAP50</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>192.168.112.99</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>SALON RETIRO 5</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>BUESCAP51</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>192.168.112.100</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>SALON RETIRO 6</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>BUESCAP52</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>192.168.112.101</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Ombu B</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>BUESCAP53</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>192.168.112.102</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Ombu A</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>BUESCAP54</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>192.168.112.103</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Martin Fierro B</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>BUESCAP55</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>192.168.112.104</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Martin Fierro A</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>BUESCAP56</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>192.168.112.105</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Poncho</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>BUESCAP57</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>192.168.112.106</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Rio DE LA PLATA</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>libre</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>192.168.112.107</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>192.168.112.108</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
id en put vsz
</commit_message>
<xml_diff>
--- a/media/output.xlsx
+++ b/media/output.xlsx
@@ -528,6 +528,16 @@
           <t>192.168.112.53</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:40:30</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>122379002563</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>SAN TELMO 4</t>
@@ -535,7 +545,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -550,6 +560,16 @@
           <t>192.168.112.54</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:7E:40</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>122379003345</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>SAN TELMO 5</t>
@@ -557,7 +577,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -572,6 +592,16 @@
           <t>192.168.112.55</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:79:00</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>122379003248</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr">
         <is>
           <t>SAN ISIDRO 1</t>
@@ -579,7 +609,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -594,6 +624,16 @@
           <t>192.168.112.56</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:7D:30</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>122379003336</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>SAN ISIDRO 2</t>
@@ -601,7 +641,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -616,6 +656,16 @@
           <t>192.168.112.57</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:3C:70</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>122379002751</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>SAN ISIDRO 3</t>
@@ -623,7 +673,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -638,6 +688,16 @@
           <t>192.168.112.58</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:3F:90</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>122379002574</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>SAN ISIDRO 4</t>
@@ -645,7 +705,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -660,6 +720,16 @@
           <t>192.168.112.59</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:3C:C0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>122379002492</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr">
         <is>
           <t>FOYER SAN ISIDRO</t>
@@ -667,7 +737,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -689,7 +759,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -711,7 +781,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -733,7 +803,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -755,7 +825,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -777,7 +847,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -799,7 +869,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -821,7 +891,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -843,7 +913,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -865,7 +935,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -887,7 +957,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -909,7 +979,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -931,7 +1001,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -953,7 +1023,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -975,7 +1045,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -997,7 +1067,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1019,7 +1089,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1034,6 +1104,16 @@
           <t>192.168.112.76</t>
         </is>
       </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:7B:60</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>122379003491</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr">
         <is>
           <t>LA PAMPA 1</t>
@@ -1041,7 +1121,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1056,6 +1136,16 @@
           <t>192.168.112.77</t>
         </is>
       </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:46:D0</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>122379002766</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr">
         <is>
           <t>LA PAMPA 2</t>
@@ -1063,7 +1153,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1078,6 +1168,16 @@
           <t>192.168.112.78</t>
         </is>
       </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:7B:30</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>122379003496</t>
+        </is>
+      </c>
       <c r="E29" t="inlineStr">
         <is>
           <t>GOLDEN 1</t>
@@ -1085,7 +1185,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1100,6 +1200,16 @@
           <t>192.168.112.79</t>
         </is>
       </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:78:50</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>122379003270</t>
+        </is>
+      </c>
       <c r="E30" t="inlineStr">
         <is>
           <t>GOLDEN 2</t>
@@ -1107,7 +1217,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1122,6 +1232,16 @@
           <t>192.168.112.80</t>
         </is>
       </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:7B:B0</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>122379003479</t>
+        </is>
+      </c>
       <c r="E31" t="inlineStr">
         <is>
           <t>CATALINAS 1</t>
@@ -1129,7 +1249,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1144,6 +1264,16 @@
           <t>192.168.112.81</t>
         </is>
       </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:7C:B0</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>122379003372</t>
+        </is>
+      </c>
       <c r="E32" t="inlineStr">
         <is>
           <t>CATALINAS 2</t>
@@ -1151,7 +1281,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1166,6 +1296,16 @@
           <t>192.168.112.82</t>
         </is>
       </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:47:00</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>122379002655</t>
+        </is>
+      </c>
       <c r="E33" t="inlineStr">
         <is>
           <t>FOYER CATALINAS</t>
@@ -1173,7 +1313,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1188,6 +1328,16 @@
           <t>192.168.112.83</t>
         </is>
       </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:3C:50</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>122379002753</t>
+        </is>
+      </c>
       <c r="E34" t="inlineStr">
         <is>
           <t>FOYER LIBERTADOR 1</t>
@@ -1195,7 +1345,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1210,6 +1360,16 @@
           <t>192.168.112.84</t>
         </is>
       </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:77:B0</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>122379003291</t>
+        </is>
+      </c>
       <c r="E35" t="inlineStr">
         <is>
           <t>FOYER LIBERTADOR 2</t>
@@ -1217,7 +1377,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1232,6 +1392,16 @@
           <t>192.168.112.85</t>
         </is>
       </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:7C:A0</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>122379003407</t>
+        </is>
+      </c>
       <c r="E36" t="inlineStr">
         <is>
           <t>FOYER LIBERTADOR 3</t>
@@ -1239,7 +1409,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1254,6 +1424,16 @@
           <t>192.168.112.86</t>
         </is>
       </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:48:00</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>122379002661</t>
+        </is>
+      </c>
       <c r="E37" t="inlineStr">
         <is>
           <t>FOYER LIBERTADOR 4</t>
@@ -1261,7 +1441,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1276,6 +1456,16 @@
           <t>192.168.112.87</t>
         </is>
       </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:7B:40</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>122379003495</t>
+        </is>
+      </c>
       <c r="E38" t="inlineStr">
         <is>
           <t>SALON LIBERTADOR 1</t>
@@ -1283,7 +1473,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1298,6 +1488,16 @@
           <t>192.168.112.88</t>
         </is>
       </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:3C:A0</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>122379002744</t>
+        </is>
+      </c>
       <c r="E39" t="inlineStr">
         <is>
           <t>SALON LIBERTADOR 2</t>
@@ -1305,7 +1505,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1320,6 +1520,16 @@
           <t>192.168.112.89</t>
         </is>
       </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:45:C0</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>122379002607</t>
+        </is>
+      </c>
       <c r="E40" t="inlineStr">
         <is>
           <t>SALON LIBERTADOR 3</t>
@@ -1327,7 +1537,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1342,6 +1552,16 @@
           <t>192.168.112.90</t>
         </is>
       </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:79:10</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>122379003247</t>
+        </is>
+      </c>
       <c r="E41" t="inlineStr">
         <is>
           <t>SALON LIBERTADOR 4</t>
@@ -1349,7 +1569,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1364,6 +1584,16 @@
           <t>192.168.112.91</t>
         </is>
       </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:7B:D0</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>122379003765</t>
+        </is>
+      </c>
       <c r="E42" t="inlineStr">
         <is>
           <t>SALON LIBERTADOR 5</t>
@@ -1371,7 +1601,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1386,6 +1616,16 @@
           <t>192.168.112.92</t>
         </is>
       </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:3C:40</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>122379002754</t>
+        </is>
+      </c>
       <c r="E43" t="inlineStr">
         <is>
           <t>SALON LIBERTADOR 6</t>
@@ -1393,7 +1633,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1408,6 +1648,16 @@
           <t>192.168.112.93</t>
         </is>
       </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:44:90</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>122379002624</t>
+        </is>
+      </c>
       <c r="E44" t="inlineStr">
         <is>
           <t>FOYER RETIRO 1</t>
@@ -1415,7 +1665,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1430,6 +1680,16 @@
           <t>192.168.112.94</t>
         </is>
       </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:7D:C0</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>122379003484</t>
+        </is>
+      </c>
       <c r="E45" t="inlineStr">
         <is>
           <t>FOYER RETIRO 2</t>
@@ -1437,7 +1697,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1452,6 +1712,16 @@
           <t>192.168.112.95</t>
         </is>
       </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:77:A0</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>122379003300</t>
+        </is>
+      </c>
       <c r="E46" t="inlineStr">
         <is>
           <t>SALON RETIRO 1</t>
@@ -1459,7 +1729,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>
@@ -1474,6 +1744,16 @@
           <t>192.168.112.96</t>
         </is>
       </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>3C:46:A1:25:7E:80</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>122379003341</t>
+        </is>
+      </c>
       <c r="E47" t="inlineStr">
         <is>
           <t>SALON RETIRO 2</t>
@@ -1481,7 +1761,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>libre</t>
+          <t>en uso</t>
         </is>
       </c>
     </row>

</xml_diff>